<commit_message>
Added a related charges writer - only includes DOJ headers + 1 additional column - writes to a separate related charges file - still need to update related charges matchers
[#169132135]

Co-authored-by: Symonne Singleton <symonne@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/related_charges.xlsx
+++ b/test_fixtures/related_charges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A092E05-6F22-5443-B0F4-8145CFD94280}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262B9026-2211-E145-B421-E17E0C9961B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="161">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -312,42 +312,6 @@
     <t>END_OF_REC</t>
   </si>
   <si>
-    <t>Case Number</t>
-  </si>
-  <si>
-    <t># of convictions on record</t>
-  </si>
-  <si>
-    <t>Superstrike Code Section(s)</t>
-  </si>
-  <si>
-    <t>PC290 Code Section(s)</t>
-  </si>
-  <si>
-    <t>PC290 Registration</t>
-  </si>
-  <si>
-    <t>Date of Conviction</t>
-  </si>
-  <si>
-    <t>Years Since This Conviction</t>
-  </si>
-  <si>
-    <t>Years Since Any Conviction</t>
-  </si>
-  <si>
-    <t># of Prop 64 convictions</t>
-  </si>
-  <si>
-    <t>Deceased</t>
-  </si>
-  <si>
-    <t>Eligibility Determination</t>
-  </si>
-  <si>
-    <t>Eligibility Reason</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -453,27 +417,6 @@
     <t>MONTHS</t>
   </si>
   <si>
-    <t>NULL  ; 140192; 140193</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>04/11/1981</t>
-  </si>
-  <si>
-    <t>38.6</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Eligible for Dismissal</t>
-  </si>
-  <si>
     <t>BIRD,BIG</t>
   </si>
   <si>
@@ -486,21 +429,6 @@
     <t xml:space="preserve">                      </t>
   </si>
   <si>
-    <t>398765; 678544</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>06/01/1979</t>
-  </si>
-  <si>
-    <t>40.4</t>
-  </si>
-  <si>
     <t>REGISTRATION</t>
   </si>
   <si>
@@ -555,43 +483,7 @@
     <t>hello</t>
   </si>
   <si>
-    <t>34.0</t>
-  </si>
-  <si>
-    <t>11/01/1985</t>
-  </si>
-  <si>
-    <t>57 years or older</t>
-  </si>
-  <si>
     <t>0</t>
-  </si>
-  <si>
-    <t># of HS 11357 convictions</t>
-  </si>
-  <si>
-    <t># of HS 11358 convictions</t>
-  </si>
-  <si>
-    <t># of HS 11359 convictions</t>
-  </si>
-  <si>
-    <t># of HS 11360 convictions</t>
-  </si>
-  <si>
-    <t>Dismiss all HS 11358 convictions</t>
-  </si>
-  <si>
-    <t>Dismiss all HS 11357 convictions</t>
-  </si>
-  <si>
-    <t>Occurred after 11/9/2016</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Possible Other P64 Charges</t>
   </si>
   <si>
     <t>186.22(A) PC-PARTICIPATE:CRIM ST GANG</t>
@@ -2461,10 +2353,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DL13"/>
+  <dimension ref="A1:CS13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AG25" sqref="AG25"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2557,21 +2449,12 @@
     <col min="94" max="94" width="15.33203125" style="1" customWidth="1"/>
     <col min="95" max="95" width="26.83203125" style="1" customWidth="1"/>
     <col min="96" max="96" width="12.5" style="1" customWidth="1"/>
-    <col min="97" max="97" width="29.6640625" style="1" customWidth="1"/>
-    <col min="98" max="100" width="24" style="1" customWidth="1"/>
-    <col min="101" max="103" width="23.6640625" style="1" customWidth="1"/>
-    <col min="104" max="104" width="12.5" style="1" customWidth="1"/>
-    <col min="105" max="105" width="23.5" style="1" customWidth="1"/>
-    <col min="106" max="106" width="23.1640625" style="1" customWidth="1"/>
-    <col min="107" max="111" width="20.5" style="1" customWidth="1"/>
-    <col min="112" max="113" width="25.83203125" style="1" customWidth="1"/>
-    <col min="114" max="114" width="52.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="35.33203125" customWidth="1"/>
+    <col min="97" max="97" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:116" s="24" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:97" s="24" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="21" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
@@ -2584,16 +2467,16 @@
       <c r="K1" s="23"/>
       <c r="L1" s="23"/>
       <c r="M1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="N1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="Q1" s="23"/>
       <c r="R1" s="23"/>
@@ -2603,7 +2486,7 @@
       <c r="V1" s="23"/>
       <c r="W1" s="23"/>
       <c r="X1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="Y1" s="23"/>
       <c r="Z1" s="23"/>
@@ -2619,15 +2502,15 @@
       <c r="AJ1" s="23"/>
       <c r="AK1" s="23"/>
       <c r="AL1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="AM1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="AN1" s="23"/>
       <c r="AO1" s="23"/>
       <c r="AP1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="AQ1" s="23"/>
       <c r="AR1" s="23"/>
@@ -2635,25 +2518,25 @@
       <c r="AT1" s="23"/>
       <c r="AU1" s="23"/>
       <c r="AV1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="AW1" s="23"/>
       <c r="AX1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="AY1" s="23"/>
       <c r="AZ1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="BA1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="BB1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="BC1" s="23"/>
       <c r="BD1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="BE1" s="23"/>
       <c r="BF1" s="23"/>
@@ -2680,99 +2563,44 @@
       <c r="CA1" s="23"/>
       <c r="CB1" s="23"/>
       <c r="CC1" s="23" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="CD1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="CE1" s="23"/>
       <c r="CF1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="CG1" s="23"/>
       <c r="CH1" s="23"/>
       <c r="CI1" s="23"/>
       <c r="CJ1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="CK1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="CL1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="CM1" s="23"/>
       <c r="CN1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="CO1" s="23"/>
       <c r="CP1" s="23"/>
       <c r="CQ1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="CR1" s="23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="CS1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="CT1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="CU1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="CV1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="CW1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="CX1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="CY1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="CZ1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DA1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DB1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DC1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DD1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DE1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DF1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DG1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DH1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DI1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DJ1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DK1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="DL1" s="23"/>
+        <v>150</v>
+      </c>
     </row>
-    <row r="2" spans="1:116" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:97" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3062,75 +2890,21 @@
         <v>94</v>
       </c>
       <c r="CS2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="CT2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="CU2" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="CV2" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="CW2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="CX2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="CY2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="CZ2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="DA2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="DB2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="DC2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="DD2" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="DE2" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="DF2" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="DG2" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="DH2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="DI2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="DJ2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="DK2" s="2" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:116" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:97" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D3" s="5">
         <v>18675309</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F3" s="5">
         <v>1008675309</v>
@@ -3143,7 +2917,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="5"/>
       <c r="N3" s="6" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="5">
@@ -3151,109 +2925,109 @@
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="6" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL3" s="18" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="AM3" s="6" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP3" s="5">
         <v>19790525</v>
       </c>
       <c r="AQ3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR3" s="6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="AS3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AT3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV3" s="6" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AW3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX3" s="6" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ3" s="18" t="s">
-        <v>192</v>
+        <v>156</v>
       </c>
       <c r="BA3" s="5">
         <v>19790525</v>
@@ -3262,16 +3036,16 @@
         <v>140189</v>
       </c>
       <c r="BC3" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD3" s="6" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="BE3" s="6" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="BF3" s="6" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="BG3" s="7"/>
       <c r="BH3" s="7"/>
@@ -3297,14 +3071,14 @@
       <c r="CB3" s="7"/>
       <c r="CC3" s="7"/>
       <c r="CD3" s="6" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="CE3" s="7"/>
       <c r="CF3" s="6" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="CG3" s="6" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH3" s="7"/>
       <c r="CI3" s="7"/>
@@ -3312,7 +3086,7 @@
       <c r="CK3" s="7"/>
       <c r="CL3" s="7"/>
       <c r="CM3" s="6" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="CN3" s="5">
         <v>23</v>
@@ -3321,40 +3095,22 @@
       <c r="CP3" s="7"/>
       <c r="CQ3" s="7"/>
       <c r="CR3" s="6" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CS3" s="7"/>
-      <c r="CT3" s="6"/>
-      <c r="CU3" s="6"/>
-      <c r="CV3" s="6"/>
-      <c r="CW3" s="6"/>
-      <c r="CX3" s="6"/>
-      <c r="CY3" s="6"/>
-      <c r="CZ3" s="6"/>
-      <c r="DA3" s="6"/>
-      <c r="DB3" s="6"/>
-      <c r="DC3" s="6"/>
-      <c r="DD3" s="6"/>
-      <c r="DE3" s="6"/>
-      <c r="DF3" s="6"/>
-      <c r="DG3" s="6"/>
-      <c r="DH3" s="7"/>
-      <c r="DI3" s="7"/>
-      <c r="DJ3" s="7"/>
-      <c r="DK3" s="7"/>
     </row>
-    <row r="4" spans="1:116" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="8" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D4" s="10">
         <v>18675309</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F4" s="10">
         <v>1008675309</v>
@@ -3367,7 +3123,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="10"/>
       <c r="N4" s="11" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="O4" s="11"/>
       <c r="P4" s="10">
@@ -3375,127 +3131,127 @@
       </c>
       <c r="Q4" s="10"/>
       <c r="R4" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL4" s="19" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="AM4" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP4" s="10">
         <v>19790601</v>
       </c>
       <c r="AQ4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR4" s="11" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="AS4" s="11" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AT4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV4" s="11" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="AW4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX4" s="11" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ4" s="19" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
       <c r="BA4" s="10">
         <v>19790601</v>
       </c>
       <c r="BB4" s="11" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="BC4" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD4" s="11" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="BE4" s="11" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="BF4" s="11" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="BG4" s="12"/>
       <c r="BH4" s="12"/>
@@ -3521,32 +3277,32 @@
       <c r="CB4" s="12"/>
       <c r="CC4" s="12"/>
       <c r="CD4" s="11" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="CE4" s="11" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="CF4" s="11" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="CG4" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH4" s="12"/>
       <c r="CI4" s="11" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="CJ4" s="11" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="CK4" s="10">
         <v>90</v>
       </c>
       <c r="CL4" s="11" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="CM4" s="11" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="CN4" s="10">
         <v>23</v>
@@ -3555,40 +3311,22 @@
       <c r="CP4" s="12"/>
       <c r="CQ4" s="12"/>
       <c r="CR4" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS4" s="12"/>
-      <c r="CT4" s="11"/>
-      <c r="CU4" s="11"/>
-      <c r="CV4" s="11"/>
-      <c r="CW4" s="11"/>
-      <c r="CX4" s="11"/>
-      <c r="CY4" s="11"/>
-      <c r="CZ4" s="11"/>
-      <c r="DA4" s="11"/>
-      <c r="DB4" s="11"/>
-      <c r="DC4" s="11"/>
-      <c r="DD4" s="11"/>
-      <c r="DE4" s="11"/>
-      <c r="DF4" s="11"/>
-      <c r="DG4" s="11"/>
-      <c r="DH4" s="12"/>
-      <c r="DI4" s="12"/>
-      <c r="DJ4" s="12"/>
-      <c r="DK4" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="CS4" s="7"/>
     </row>
-    <row r="5" spans="1:116" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="8" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D5" s="10">
         <v>18675309</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F5" s="10">
         <v>1008675309</v>
@@ -3601,7 +3339,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="10"/>
       <c r="N5" s="11" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="10">
@@ -3609,109 +3347,109 @@
       </c>
       <c r="Q5" s="10"/>
       <c r="R5" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL5" s="19" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="AM5" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP5" s="10">
         <v>19810410</v>
       </c>
       <c r="AQ5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR5" s="11" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="AS5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AT5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV5" s="11" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AW5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX5" s="11" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ5" s="19" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="BA5" s="10">
         <v>19810410</v>
@@ -3720,14 +3458,14 @@
         <v>140190</v>
       </c>
       <c r="BC5" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD5" s="19" t="s">
-        <v>189</v>
+        <v>153</v>
       </c>
       <c r="BE5" s="11"/>
       <c r="BF5" s="11" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="BG5" s="12"/>
       <c r="BH5" s="12"/>
@@ -3754,13 +3492,13 @@
       <c r="CC5" s="12"/>
       <c r="CD5" s="12"/>
       <c r="CE5" s="11" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="CF5" s="11" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="CG5" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH5" s="12"/>
       <c r="CI5" s="12"/>
@@ -3768,7 +3506,7 @@
       <c r="CK5" s="12"/>
       <c r="CL5" s="12"/>
       <c r="CM5" s="11" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="CN5" s="10">
         <v>25</v>
@@ -3777,40 +3515,22 @@
       <c r="CP5" s="12"/>
       <c r="CQ5" s="12"/>
       <c r="CR5" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS5" s="12"/>
-      <c r="CT5" s="11"/>
-      <c r="CU5" s="11"/>
-      <c r="CV5" s="11"/>
-      <c r="CW5" s="11"/>
-      <c r="CX5" s="11"/>
-      <c r="CY5" s="11"/>
-      <c r="CZ5" s="11"/>
-      <c r="DA5" s="11"/>
-      <c r="DB5" s="11"/>
-      <c r="DC5" s="11"/>
-      <c r="DD5" s="11"/>
-      <c r="DE5" s="11"/>
-      <c r="DF5" s="11"/>
-      <c r="DG5" s="11"/>
-      <c r="DH5" s="12"/>
-      <c r="DI5" s="12"/>
-      <c r="DJ5" s="12"/>
-      <c r="DK5" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="CS5" s="7"/>
     </row>
-    <row r="6" spans="1:116" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="8" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D6" s="10">
         <v>18675309</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F6" s="10">
         <v>1008675309</v>
@@ -3823,7 +3543,7 @@
       <c r="L6" s="11"/>
       <c r="M6" s="10"/>
       <c r="N6" s="11" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="10">
@@ -3831,109 +3551,109 @@
       </c>
       <c r="Q6" s="10"/>
       <c r="R6" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL6" s="19" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="AM6" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP6" s="10">
         <v>19810410</v>
       </c>
       <c r="AQ6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR6" s="11" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="AS6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AT6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV6" s="11" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AW6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX6" s="11" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ6" s="19" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="BA6" s="10">
         <v>19810410</v>
@@ -3942,14 +3662,14 @@
         <v>140190</v>
       </c>
       <c r="BC6" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD6" s="11" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="BE6" s="11"/>
       <c r="BF6" s="11" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="BG6" s="12"/>
       <c r="BH6" s="12"/>
@@ -3976,13 +3696,13 @@
       <c r="CC6" s="12"/>
       <c r="CD6" s="12"/>
       <c r="CE6" s="11" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="CF6" s="11" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="CG6" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH6" s="12"/>
       <c r="CI6" s="12"/>
@@ -3990,7 +3710,7 @@
       <c r="CK6" s="12"/>
       <c r="CL6" s="12"/>
       <c r="CM6" s="11" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="CN6" s="10">
         <v>25</v>
@@ -3999,43 +3719,25 @@
       <c r="CP6" s="12"/>
       <c r="CQ6" s="12"/>
       <c r="CR6" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS6" s="12"/>
-      <c r="CT6" s="11"/>
-      <c r="CU6" s="11"/>
-      <c r="CV6" s="11"/>
-      <c r="CW6" s="11"/>
-      <c r="CX6" s="11"/>
-      <c r="CY6" s="11"/>
-      <c r="CZ6" s="11"/>
-      <c r="DA6" s="11"/>
-      <c r="DB6" s="11"/>
-      <c r="DC6" s="11"/>
-      <c r="DD6" s="11"/>
-      <c r="DE6" s="11"/>
-      <c r="DF6" s="11"/>
-      <c r="DG6" s="11"/>
-      <c r="DH6" s="12"/>
-      <c r="DI6" s="12"/>
-      <c r="DJ6" s="12"/>
-      <c r="DK6" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="CS6" s="7"/>
     </row>
-    <row r="7" spans="1:116" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="b">
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D7" s="10">
         <v>18675309</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F7" s="10">
         <v>1008675309</v>
@@ -4048,7 +3750,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="10"/>
       <c r="N7" s="11" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="10">
@@ -4056,109 +3758,109 @@
       </c>
       <c r="Q7" s="10"/>
       <c r="R7" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL7" s="19" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="AM7" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP7" s="10">
         <v>19810411</v>
       </c>
       <c r="AQ7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR7" s="11" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="AS7" s="11" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AT7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV7" s="11" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="AW7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX7" s="11" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ7" s="19" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="BA7" s="10">
         <v>19810411</v>
@@ -4167,16 +3869,16 @@
         <v>140192</v>
       </c>
       <c r="BC7" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD7" s="19" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="BE7" s="11" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="BF7" s="11" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="BG7" s="12"/>
       <c r="BH7" s="12"/>
@@ -4202,14 +3904,14 @@
       <c r="CB7" s="12"/>
       <c r="CC7" s="12"/>
       <c r="CD7" s="11" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="CE7" s="12"/>
       <c r="CF7" s="11" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="CG7" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH7" s="12"/>
       <c r="CI7" s="12"/>
@@ -4217,7 +3919,7 @@
       <c r="CK7" s="12"/>
       <c r="CL7" s="12"/>
       <c r="CM7" s="11" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="CN7" s="10">
         <v>25</v>
@@ -4226,42 +3928,24 @@
       <c r="CP7" s="12"/>
       <c r="CQ7" s="12"/>
       <c r="CR7" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS7" s="12"/>
-      <c r="CT7" s="11"/>
-      <c r="CU7" s="11"/>
-      <c r="CV7" s="11"/>
-      <c r="CW7" s="11"/>
-      <c r="CX7" s="11"/>
-      <c r="CY7" s="11"/>
-      <c r="CZ7" s="11"/>
-      <c r="DA7" s="11"/>
-      <c r="DB7" s="11"/>
-      <c r="DC7" s="11"/>
-      <c r="DD7" s="11"/>
-      <c r="DE7" s="11"/>
-      <c r="DF7" s="11"/>
-      <c r="DG7" s="11"/>
-      <c r="DH7" s="12"/>
-      <c r="DI7" s="12"/>
-      <c r="DJ7" s="12"/>
-      <c r="DK7" s="25" t="s">
-        <v>195</v>
+        <v>96</v>
+      </c>
+      <c r="CS7" s="25" t="s">
+        <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:116" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="8" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D8" s="10">
         <v>18675309</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F8" s="10">
         <v>1008675309</v>
@@ -4274,7 +3958,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="10"/>
       <c r="N8" s="11" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="O8" s="11"/>
       <c r="P8" s="10">
@@ -4282,109 +3966,109 @@
       </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL8" s="19" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="AM8" s="11" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP8" s="10">
         <v>19810411</v>
       </c>
       <c r="AQ8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR8" s="11" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="AS8" s="11" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AT8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV8" s="11" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="AW8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX8" s="19" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ8" s="19" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="BA8" s="10">
         <v>19810411</v>
@@ -4393,16 +4077,16 @@
         <v>140193</v>
       </c>
       <c r="BC8" s="11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD8" s="11" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="BE8" s="11" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="BF8" s="11" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="BG8" s="12"/>
       <c r="BH8" s="12"/>
@@ -4428,32 +4112,32 @@
       <c r="CB8" s="12"/>
       <c r="CC8" s="12"/>
       <c r="CD8" s="19" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="CE8" s="11" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="CF8" s="11" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="CG8" s="11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH8" s="12"/>
       <c r="CI8" s="11" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="CJ8" s="11" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="CK8" s="10">
         <v>6</v>
       </c>
       <c r="CL8" s="11" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="CM8" s="11" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="CN8" s="10">
         <v>25</v>
@@ -4462,74 +4146,22 @@
       <c r="CP8" s="12"/>
       <c r="CQ8" s="12"/>
       <c r="CR8" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS8" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="CT8" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="CU8" s="11"/>
-      <c r="CV8" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="CW8" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="CX8" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="CY8" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="CZ8" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="DA8" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="DB8" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="DC8" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="DD8" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="DE8" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="DF8" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="DG8" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="DH8" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="DI8" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="DJ8" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="DK8" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="CS8" s="7"/>
     </row>
-    <row r="9" spans="1:116" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="13" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D9" s="15">
         <v>17954908</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F9" s="16">
         <v>8690594867</v>
@@ -4542,7 +4174,7 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="O9" s="16"/>
       <c r="P9" s="15">
@@ -4550,109 +4182,109 @@
       </c>
       <c r="Q9" s="15"/>
       <c r="R9" s="16" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="S9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL9" s="20" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="AM9" s="16" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP9" s="15">
         <v>19790525</v>
       </c>
       <c r="AQ9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR9" s="16" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="AS9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AT9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV9" s="16" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AW9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX9" s="16" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ9" s="20" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="BA9" s="15">
         <v>19790525</v>
@@ -4661,16 +4293,16 @@
         <v>987340</v>
       </c>
       <c r="BC9" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD9" s="16" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="BE9" s="16" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="BF9" s="16" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="BG9" s="17"/>
       <c r="BH9" s="17"/>
@@ -4696,14 +4328,14 @@
       <c r="CB9" s="17"/>
       <c r="CC9" s="17"/>
       <c r="CD9" s="16" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="CE9" s="16"/>
       <c r="CF9" s="16" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="CG9" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH9" s="17"/>
       <c r="CI9" s="16"/>
@@ -4711,7 +4343,7 @@
       <c r="CK9" s="15"/>
       <c r="CL9" s="16"/>
       <c r="CM9" s="16" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="CN9" s="17">
         <v>23</v>
@@ -4720,40 +4352,22 @@
       <c r="CP9" s="17"/>
       <c r="CQ9" s="17"/>
       <c r="CR9" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS9" s="15"/>
-      <c r="CT9" s="16"/>
-      <c r="CU9" s="16"/>
-      <c r="CV9" s="16"/>
-      <c r="CW9" s="16"/>
-      <c r="CX9" s="16"/>
-      <c r="CY9" s="16"/>
-      <c r="CZ9" s="16"/>
-      <c r="DA9" s="16"/>
-      <c r="DB9" s="16"/>
-      <c r="DC9" s="16"/>
-      <c r="DD9" s="16"/>
-      <c r="DE9" s="16"/>
-      <c r="DF9" s="16"/>
-      <c r="DG9" s="16"/>
-      <c r="DH9" s="16"/>
-      <c r="DI9" s="16"/>
-      <c r="DJ9" s="16"/>
-      <c r="DK9" s="16"/>
+        <v>96</v>
+      </c>
+      <c r="CS9" s="16"/>
     </row>
-    <row r="10" spans="1:116" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="13" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D10" s="15">
         <v>17954908</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F10" s="16">
         <v>8690594867</v>
@@ -4766,7 +4380,7 @@
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
       <c r="N10" s="16" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="O10" s="16"/>
       <c r="P10" s="15">
@@ -4774,109 +4388,109 @@
       </c>
       <c r="Q10" s="15"/>
       <c r="R10" s="16" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="S10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL10" s="20" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="AM10" s="16" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP10" s="15">
         <v>19790601</v>
       </c>
       <c r="AQ10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR10" s="16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="AS10" s="16" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AT10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV10" s="16" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="AW10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX10" s="16" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ10" s="20" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="BA10" s="15">
         <v>19790601</v>
@@ -4885,16 +4499,16 @@
         <v>398765</v>
       </c>
       <c r="BC10" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD10" s="16" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="BE10" s="16" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="BF10" s="16" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="BG10" s="17"/>
       <c r="BH10" s="17"/>
@@ -4920,32 +4534,32 @@
       <c r="CB10" s="17"/>
       <c r="CC10" s="17"/>
       <c r="CD10" s="16" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="CE10" s="16" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="CF10" s="16" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="CG10" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH10" s="17"/>
       <c r="CI10" s="16" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="CJ10" s="16" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="CK10" s="15">
         <v>90</v>
       </c>
       <c r="CL10" s="16" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="CM10" s="16" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="CN10" s="17">
         <v>23</v>
@@ -4954,74 +4568,22 @@
       <c r="CP10" s="17"/>
       <c r="CQ10" s="17"/>
       <c r="CR10" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS10" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="CT10" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="CU10" s="16"/>
-      <c r="CV10" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="CW10" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="CX10" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="CY10" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="CZ10" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="DA10" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="DB10" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="DC10" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="DD10" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="DE10" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="DF10" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="DG10" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="DH10" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="DI10" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="DJ10" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="DK10" s="16"/>
+        <v>96</v>
+      </c>
+      <c r="CS10" s="16"/>
     </row>
-    <row r="11" spans="1:116" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="13" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D11" s="15">
         <v>17954908</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F11" s="16">
         <v>8690594867</v>
@@ -5034,7 +4596,7 @@
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="O11" s="16"/>
       <c r="P11" s="15">
@@ -5042,109 +4604,109 @@
       </c>
       <c r="Q11" s="15"/>
       <c r="R11" s="16" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="S11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL11" s="20" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="AM11" s="16" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP11" s="15">
         <v>19790601</v>
       </c>
       <c r="AQ11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR11" s="16" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="AS11" s="16" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AT11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV11" s="16" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="AW11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX11" s="16" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ11" s="20" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="BA11" s="15">
         <v>19790601</v>
@@ -5153,14 +4715,14 @@
         <v>678544</v>
       </c>
       <c r="BC11" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD11" s="16" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="BE11" s="16"/>
       <c r="BF11" s="16" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="BG11" s="17"/>
       <c r="BH11" s="17"/>
@@ -5187,11 +4749,11 @@
       <c r="CC11" s="17"/>
       <c r="CD11" s="16"/>
       <c r="CE11" s="16" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="CF11" s="16"/>
       <c r="CG11" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH11" s="17"/>
       <c r="CI11" s="16"/>
@@ -5199,7 +4761,7 @@
       <c r="CK11" s="15"/>
       <c r="CL11" s="16"/>
       <c r="CM11" s="16" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="CN11" s="17">
         <v>23</v>
@@ -5208,40 +4770,22 @@
       <c r="CP11" s="17"/>
       <c r="CQ11" s="17"/>
       <c r="CR11" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS11" s="15"/>
-      <c r="CT11" s="16"/>
-      <c r="CU11" s="16"/>
-      <c r="CV11" s="16"/>
-      <c r="CW11" s="16"/>
-      <c r="CX11" s="16"/>
-      <c r="CY11" s="16"/>
-      <c r="CZ11" s="16"/>
-      <c r="DA11" s="16"/>
-      <c r="DB11" s="16"/>
-      <c r="DC11" s="16"/>
-      <c r="DD11" s="16"/>
-      <c r="DE11" s="16"/>
-      <c r="DF11" s="16"/>
-      <c r="DG11" s="16"/>
-      <c r="DH11" s="16"/>
-      <c r="DI11" s="16"/>
-      <c r="DJ11" s="16"/>
-      <c r="DK11" s="16"/>
+        <v>96</v>
+      </c>
+      <c r="CS11" s="16"/>
     </row>
-    <row r="12" spans="1:116" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="13" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D12" s="15">
         <v>17954908</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F12" s="16">
         <v>8690594867</v>
@@ -5254,7 +4798,7 @@
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
       <c r="N12" s="16" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="O12" s="16"/>
       <c r="P12" s="15">
@@ -5262,109 +4806,109 @@
       </c>
       <c r="Q12" s="15"/>
       <c r="R12" s="16" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="S12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL12" s="20" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="AM12" s="16" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP12" s="15">
         <v>19851101</v>
       </c>
       <c r="AQ12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR12" s="16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="AS12" s="16" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AT12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV12" s="16" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="AW12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX12" s="16" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ12" s="20" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="BA12" s="15">
         <v>19851101</v>
@@ -5373,16 +4917,16 @@
         <v>398765</v>
       </c>
       <c r="BC12" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD12" s="16" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="BE12" s="16" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="BF12" s="16" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="BG12" s="17"/>
       <c r="BH12" s="17"/>
@@ -5408,32 +4952,32 @@
       <c r="CB12" s="17"/>
       <c r="CC12" s="17"/>
       <c r="CD12" s="16" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="CE12" s="16" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="CF12" s="16" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="CG12" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH12" s="17"/>
       <c r="CI12" s="16" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="CJ12" s="16" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="CK12" s="15">
         <v>90</v>
       </c>
       <c r="CL12" s="16" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="CM12" s="16" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="CN12" s="17">
         <v>24</v>
@@ -5442,74 +4986,22 @@
       <c r="CP12" s="17"/>
       <c r="CQ12" s="17"/>
       <c r="CR12" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS12" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="CT12" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="CU12" s="16"/>
-      <c r="CV12" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="CW12" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="CX12" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="CY12" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="CZ12" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="DA12" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="DB12" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="DC12" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="DD12" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="DE12" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="DF12" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="DG12" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="DH12" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="DI12" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="DJ12" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="DK12" s="16"/>
+        <v>96</v>
+      </c>
+      <c r="CS12" s="16"/>
     </row>
-    <row r="13" spans="1:116" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="13" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D13" s="15">
         <v>17954908</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F13" s="16">
         <v>8690594867</v>
@@ -5522,7 +5014,7 @@
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="O13" s="16"/>
       <c r="P13" s="15">
@@ -5530,109 +5022,109 @@
       </c>
       <c r="Q13" s="15"/>
       <c r="R13" s="16" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="S13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="T13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="W13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Z13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AA13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AC13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AD13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AF13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AG13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AI13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AJ13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AL13" s="20" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="AM13" s="16" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AN13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AO13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AP13" s="15">
         <v>19851101</v>
       </c>
       <c r="AQ13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AR13" s="16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="AS13" s="16" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AT13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AU13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AV13" s="16" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AW13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AX13" s="16" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AY13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AZ13" s="20" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="BA13" s="15">
         <v>19851101</v>
@@ -5641,13 +5133,13 @@
         <v>678544</v>
       </c>
       <c r="BC13" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="BD13" s="16" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="BE13" s="16" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="BF13" s="16"/>
       <c r="BG13" s="17"/>
@@ -5674,28 +5166,28 @@
       <c r="CB13" s="17"/>
       <c r="CC13" s="17"/>
       <c r="CD13" s="16" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="CE13" s="16"/>
       <c r="CF13" s="16" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="CG13" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="CH13" s="17"/>
       <c r="CI13" s="16"/>
       <c r="CJ13" s="16" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="CK13" s="15">
         <v>10</v>
       </c>
       <c r="CL13" s="16" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="CM13" s="16" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="CN13" s="17">
         <v>23</v>
@@ -5704,27 +5196,9 @@
       <c r="CP13" s="17"/>
       <c r="CQ13" s="17"/>
       <c r="CR13" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS13" s="15"/>
-      <c r="CT13" s="16"/>
-      <c r="CU13" s="16"/>
-      <c r="CV13" s="16"/>
-      <c r="CW13" s="16"/>
-      <c r="CX13" s="16"/>
-      <c r="CY13" s="16"/>
-      <c r="CZ13" s="16"/>
-      <c r="DA13" s="16"/>
-      <c r="DB13" s="16"/>
-      <c r="DC13" s="16"/>
-      <c r="DD13" s="16"/>
-      <c r="DE13" s="16"/>
-      <c r="DF13" s="16"/>
-      <c r="DG13" s="16"/>
-      <c r="DH13" s="16"/>
-      <c r="DI13" s="16"/>
-      <c r="DJ13" s="16"/>
-      <c r="DK13" s="16"/>
+        <v>96</v>
+      </c>
+      <c r="CS13" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Update related charge matcher to use SFDA codes
Co-authored-by: Symonne Singleton <symonne@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/related_charges.xlsx
+++ b/test_fixtures/related_charges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262B9026-2211-E145-B421-E17E0C9961B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EB2FB7-633F-C14F-8B1D-8C40CF02084E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="160">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -505,9 +505,6 @@
   </si>
   <si>
     <t>Potentially Eligible</t>
-  </si>
-  <si>
-    <t>466 PC-PARTICIPATE:CRIM ST GANG</t>
   </si>
 </sst>
 </file>
@@ -2356,7 +2353,7 @@
   <dimension ref="A1:CS13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3872,7 +3869,7 @@
         <v>95</v>
       </c>
       <c r="BD7" s="19" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="BE7" s="11" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Add arrests for related charges
- Add column for all arrests in related charges cycle in CSV
- Created notion of 'Cycles' and 'Steps' on a Subject, for use in future
refactors

Co-authored-by: Symonne Singleton <symonne@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/related_charges.xlsx
+++ b/test_fixtures/related_charges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EB2FB7-633F-C14F-8B1D-8C40CF02084E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F798E0AC-4A80-874E-9FB7-8536FE290680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="162">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -505,6 +505,12 @@
   </si>
   <si>
     <t>Potentially Eligible</t>
+  </si>
+  <si>
+    <t>Other Charges in Arrest</t>
+  </si>
+  <si>
+    <t>186.22(A) PC; 11358 HS</t>
   </si>
 </sst>
 </file>
@@ -2350,10 +2356,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CS13"/>
+  <dimension ref="A1:CT13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="CT7" sqref="CT7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2447,9 +2453,10 @@
     <col min="95" max="95" width="26.83203125" style="1" customWidth="1"/>
     <col min="96" max="96" width="12.5" style="1" customWidth="1"/>
     <col min="97" max="97" width="35.33203125" customWidth="1"/>
+    <col min="98" max="98" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97" s="24" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:98" s="24" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="21" t="s">
         <v>151</v>
       </c>
@@ -2596,8 +2603,11 @@
       <c r="CS1" s="23" t="s">
         <v>150</v>
       </c>
+      <c r="CT1" s="23" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="2" spans="1:97" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:98" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2889,8 +2899,11 @@
       <c r="CS2" s="2" t="s">
         <v>158</v>
       </c>
+      <c r="CT2" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="3" spans="1:97" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:98" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>95</v>
       </c>
@@ -3095,8 +3108,9 @@
         <v>96</v>
       </c>
       <c r="CS3" s="7"/>
+      <c r="CT3" s="7"/>
     </row>
-    <row r="4" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:98" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="8" t="s">
         <v>95</v>
       </c>
@@ -3311,8 +3325,9 @@
         <v>96</v>
       </c>
       <c r="CS4" s="7"/>
+      <c r="CT4" s="7"/>
     </row>
-    <row r="5" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:98" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="8" t="s">
         <v>95</v>
       </c>
@@ -3515,8 +3530,9 @@
         <v>96</v>
       </c>
       <c r="CS5" s="7"/>
+      <c r="CT5" s="7"/>
     </row>
-    <row r="6" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:98" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="8" t="s">
         <v>95</v>
       </c>
@@ -3661,7 +3677,7 @@
       <c r="BC6" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="BD6" s="11" t="s">
+      <c r="BD6" s="19" t="s">
         <v>122</v>
       </c>
       <c r="BE6" s="11"/>
@@ -3719,8 +3735,9 @@
         <v>96</v>
       </c>
       <c r="CS6" s="7"/>
+      <c r="CT6" s="7"/>
     </row>
-    <row r="7" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:98" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="b">
         <v>1</v>
       </c>
@@ -3930,8 +3947,11 @@
       <c r="CS7" s="25" t="s">
         <v>159</v>
       </c>
+      <c r="CT7" s="25" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="8" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:98" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="8" t="s">
         <v>95</v>
       </c>
@@ -4146,8 +4166,9 @@
         <v>96</v>
       </c>
       <c r="CS8" s="7"/>
+      <c r="CT8" s="7"/>
     </row>
-    <row r="9" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:98" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="13" t="s">
         <v>95</v>
       </c>
@@ -4352,8 +4373,9 @@
         <v>96</v>
       </c>
       <c r="CS9" s="16"/>
+      <c r="CT9" s="16"/>
     </row>
-    <row r="10" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:98" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="13" t="s">
         <v>95</v>
       </c>
@@ -4568,8 +4590,9 @@
         <v>96</v>
       </c>
       <c r="CS10" s="16"/>
+      <c r="CT10" s="16"/>
     </row>
-    <row r="11" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:98" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="13" t="s">
         <v>95</v>
       </c>
@@ -4770,8 +4793,9 @@
         <v>96</v>
       </c>
       <c r="CS11" s="16"/>
+      <c r="CT11" s="16"/>
     </row>
-    <row r="12" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:98" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="13" t="s">
         <v>95</v>
       </c>
@@ -4986,8 +5010,9 @@
         <v>96</v>
       </c>
       <c r="CS12" s="16"/>
+      <c r="CT12" s="16"/>
     </row>
-    <row r="13" spans="1:97" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:98" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="13" t="s">
         <v>95</v>
       </c>
@@ -5196,6 +5221,7 @@
         <v>96</v>
       </c>
       <c r="CS13" s="16"/>
+      <c r="CT13" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>